<commit_message>
Updated METS header, pymets imports, etc.
</commit_message>
<xml_diff>
--- a/NLP/PII/PII_list_and_patterns.xlsx
+++ b/NLP/PII/PII_list_and_patterns.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\PII\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\GitHub\tomes_tool\NLP\PII\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="20490" windowHeight="8655"/>
+    <workbookView xWindow="0" yWindow="6750" windowWidth="20490" windowHeight="8655"/>
   </bookViews>
   <sheets>
     <sheet name="20170105" sheetId="3" r:id="rId1"/>
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nitin:</t>
         </r>
@@ -78,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 You need to also match HTML "mailto:" emails.</t>
@@ -378,9 +378,6 @@
     <t>Patient Health Information</t>
   </si>
   <si>
-    <t>This is similar to Sensitive Document, in that trying to identify this information relates more to keyword searching rather than patter matching via regular expresions.</t>
-  </si>
-  <si>
     <t>Documents of a confidential or sensitive nature.</t>
   </si>
   <si>
@@ -418,13 +415,16 @@
   </si>
   <si>
     <t>The ones not matching are all due to odd tokenization a la "971-99-0994 949" where I'd have expected the last 3 digits to be part of the next token.</t>
+  </si>
+  <si>
+    <t>This is similar to Sensitive Document, in that trying to identify this information relates more to keyword searching rather than pattern matching via regular expresions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,19 +459,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -626,13 +613,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -965,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1031,7 +1018,7 @@
         <v>PII.sensitive_document</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>50</v>
@@ -1071,13 +1058,13 @@
         <v>PII.patient_health_information</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
@@ -1104,7 +1091,7 @@
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="20" t="str">
         <f t="shared" si="0"/>
@@ -1117,7 +1104,7 @@
         <v>52</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -1144,7 +1131,7 @@
     </row>
     <row r="9" spans="1:8" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="20" t="str">
         <f t="shared" si="0"/>
@@ -1240,19 +1227,19 @@
         <v>63</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>87</v>
-      </c>
       <c r="F1" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1291,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1310,7 +1297,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="34">
         <v>4</v>
@@ -1349,11 +1336,11 @@
         <v>78</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="34"/>
       <c r="D9" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1361,11 +1348,11 @@
         <v>68</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1380,7 +1367,7 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>